<commit_message>
Update Excel template for better A4 printing
</commit_message>
<xml_diff>
--- a/Truck_Load_Record_Template.xlsx
+++ b/Truck_Load_Record_Template.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lasikaharshana/Desktop/driver-schedule-backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4951ED08-35A4-5442-ACC9-6A2F6CBBC76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCF6103-7173-C84E-9F11-588D989E8FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="980" windowWidth="27640" windowHeight="15880" xr2:uid="{13A8B1D5-2B2F-774D-87AF-E72A5CEF18C2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{13A8B1D5-2B2F-774D-87AF-E72A5CEF18C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$N$40</definedName>
+  </definedNames>
   <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -364,7 +367,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -398,24 +401,41 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -437,25 +457,11 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -792,11 +798,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFBED206-7EB8-C842-BB08-8300413F17A8}">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:N4"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -812,26 +820,26 @@
     <col min="11" max="11" width="17.5" customWidth="1"/>
     <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="3.83203125" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" customWidth="1"/>
+    <col min="14" max="14" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
     </row>
     <row r="2" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -849,67 +857,67 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="26" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="25"/>
-    </row>
-    <row r="4" spans="1:14" ht="18" x14ac:dyDescent="0.2">
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="32"/>
+    </row>
+    <row r="4" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26" t="s">
+      <c r="B4" s="30"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="29"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="36"/>
+    </row>
+    <row r="5" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18" t="s">
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
@@ -927,670 +935,660 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:14" ht="25" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+    <row r="7" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+    </row>
+    <row r="8" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
       <c r="E8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
       <c r="I8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="21"/>
+      <c r="K8" s="27"/>
       <c r="L8" s="8"/>
-      <c r="M8" s="20" t="s">
+      <c r="M8" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="20"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
+      <c r="N8" s="21"/>
+    </row>
+    <row r="9" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
       <c r="I9" s="9"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+    </row>
+    <row r="10" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
       <c r="L10" s="2"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+    </row>
+    <row r="11" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
       <c r="E11" s="10"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+    </row>
+    <row r="12" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="10"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
       <c r="I12" s="10"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+    </row>
+    <row r="13" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="10"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="30"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+    </row>
+    <row r="14" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+    </row>
+    <row r="15" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="10"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
       <c r="L15" s="2"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+    </row>
+    <row r="16" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
       <c r="L16" s="2"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="31" t="s">
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+    </row>
+    <row r="17" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
       <c r="I17" s="11"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
       <c r="L17" s="12"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-    </row>
-    <row r="18" spans="1:14" ht="25" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+    </row>
+    <row r="18" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+    </row>
+    <row r="19" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
       <c r="E19" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="F19" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
       <c r="I19" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="21" t="s">
+      <c r="J19" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="K19" s="21"/>
+      <c r="K19" s="27"/>
       <c r="L19" s="8"/>
-      <c r="M19" s="20" t="s">
+      <c r="M19" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="N19" s="20"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="30"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
+      <c r="N19" s="21"/>
+    </row>
+    <row r="20" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
       <c r="E20" s="9"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
       <c r="I20" s="9"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
       <c r="L20" s="14"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+    </row>
+    <row r="21" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="22"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
       <c r="E21" s="10"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
       <c r="L21" s="14"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+    </row>
+    <row r="22" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
       <c r="E22" s="10"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
       <c r="I22" s="10"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
       <c r="L22" s="14"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+    </row>
+    <row r="23" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
       <c r="E23" s="10"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
       <c r="I23" s="10"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="30"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
       <c r="L23" s="14"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="30"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+    </row>
+    <row r="24" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
       <c r="E24" s="10"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
       <c r="I24" s="10"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
       <c r="L24" s="14"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+    </row>
+    <row r="25" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
       <c r="E25" s="10"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
       <c r="I25" s="10"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="30"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
       <c r="L25" s="14"/>
-      <c r="M25" s="30"/>
-      <c r="N25" s="30"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+    </row>
+    <row r="26" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
       <c r="E26" s="10"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
       <c r="I26" s="10"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
       <c r="L26" s="14"/>
-      <c r="M26" s="30"/>
-      <c r="N26" s="30"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="30"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+    </row>
+    <row r="27" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
       <c r="E27" s="10"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
       <c r="I27" s="10"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="30"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
       <c r="L27" s="14"/>
-      <c r="M27" s="30"/>
-      <c r="N27" s="30"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="30"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+    </row>
+    <row r="28" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="22"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
       <c r="E28" s="10"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
       <c r="I28" s="10"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="30"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
       <c r="L28" s="14"/>
-      <c r="M28" s="30"/>
-      <c r="N28" s="30"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="30"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+    </row>
+    <row r="29" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="22"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
       <c r="E29" s="10"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
       <c r="I29" s="10"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
       <c r="L29" s="14"/>
-      <c r="M29" s="30"/>
-      <c r="N29" s="30"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+    </row>
+    <row r="30" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
       <c r="E30" s="10"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
       <c r="I30" s="10"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
       <c r="L30" s="14"/>
-      <c r="M30" s="30"/>
-      <c r="N30" s="30"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="22"/>
     </row>
     <row r="31" spans="1:14" ht="25" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="20" t="s">
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="25"/>
+      <c r="N31" s="25"/>
+    </row>
+    <row r="32" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20" t="s">
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="20"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="20" t="s">
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+    </row>
+    <row r="33" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="30"/>
-      <c r="M33" s="30"/>
-      <c r="N33" s="30"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="20" t="s">
+      <c r="B33" s="21"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="22"/>
+    </row>
+    <row r="34" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="30"/>
-      <c r="N34" s="30"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A35" s="20" t="s">
+      <c r="B34" s="21"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
+    </row>
+    <row r="35" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="20"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="30"/>
-      <c r="N35" s="30"/>
-    </row>
-    <row r="36" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="B35" s="21"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
+    </row>
+    <row r="36" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="37" t="s">
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F36" s="37"/>
-      <c r="G36" s="36" t="s">
+      <c r="F36" s="24"/>
+      <c r="G36" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="H36" s="36"/>
+      <c r="H36" s="23"/>
       <c r="I36" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-      <c r="M36" s="30"/>
-      <c r="N36" s="30"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
     </row>
     <row r="37" spans="1:14" ht="18" x14ac:dyDescent="0.2">
-      <c r="A37" s="32" t="s">
+      <c r="A37" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="32"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="32"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
     </row>
     <row r="38" spans="1:14" ht="28" x14ac:dyDescent="0.2">
-      <c r="A38" s="33" t="s">
+      <c r="A38" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="33"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="33"/>
-      <c r="K38" s="33"/>
-      <c r="L38" s="33"/>
-      <c r="M38" s="33"/>
-      <c r="N38" s="33"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="18"/>
     </row>
     <row r="39" spans="1:14" ht="18" x14ac:dyDescent="0.2">
-      <c r="A39" s="34" t="s">
+      <c r="A39" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
-      <c r="K39" s="34"/>
-      <c r="L39" s="34"/>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
     </row>
     <row r="40" spans="1:14" ht="18" x14ac:dyDescent="0.2">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="35"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="35"/>
-      <c r="J40" s="35"/>
-      <c r="K40" s="35"/>
-      <c r="L40" s="35"/>
-      <c r="M40" s="35"/>
-      <c r="N40" s="35"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="119">
-    <mergeCell ref="A37:N37"/>
-    <mergeCell ref="A38:N38"/>
-    <mergeCell ref="A39:N39"/>
-    <mergeCell ref="A40:N40"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="H35:N35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="J36:N36"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H33:N33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="H34:N34"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="A31:N31"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="H32:N32"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="A7:N7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="I4:N4"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="M14:N14"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="J20:K20"/>
@@ -1608,53 +1606,64 @@
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="J19:K19"/>
     <mergeCell ref="M19:N19"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="G5:N5"/>
-    <mergeCell ref="A7:N7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="I3:N3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="I4:N4"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="H33:N33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="H34:N34"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="A31:N31"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="H32:N32"/>
+    <mergeCell ref="A37:N37"/>
+    <mergeCell ref="A38:N38"/>
+    <mergeCell ref="A39:N39"/>
+    <mergeCell ref="A40:N40"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="H35:N35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="J36:N36"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.51624999999999999" bottom="0.55722222222222217" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="59" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>